<commit_message>
I should be committing more frequently. Finally have a readme though.
</commit_message>
<xml_diff>
--- a/Hardware/TransmitterPCB/V1/BOM.xlsx
+++ b/Hardware/TransmitterPCB/V1/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02be13960f358456/Classes/College/Semester 6/Research Project/Hardware/TransmitterPCB/V1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawaiz\SkyDrive\Classes\College\Semester 6\Research Project\Hardware\TransmitterPCB\V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -419,9 +419,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00000_);_(&quot;$&quot;* \(#,##0.00000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,7 +461,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -746,24 +746,24 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="153.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="153.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -795,7 +795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -819,7 +819,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -852,7 +852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -885,7 +885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -918,7 +918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -951,7 +951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -984,7 +984,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>93</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>95</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>119</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>20.260300000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H25" s="2" t="s">
         <v>128</v>
       </c>

</xml_diff>